<commit_message>
plan import with variants
</commit_message>
<xml_diff>
--- a/deployments/hsphere_plan_data.xlsx
+++ b/deployments/hsphere_plan_data.xlsx
@@ -11,12 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>plan_name</t>
   </si>
   <si>
-    <t>plan_price</t>
+    <t>plan_price_monthly</t>
+  </si>
+  <si>
+    <t>plan_price_semi_annual</t>
+  </si>
+  <si>
+    <t>plan_price_annual</t>
   </si>
   <si>
     <t>plan_duration</t>
@@ -31,10 +37,13 @@
     <t>opspi_account_id</t>
   </si>
   <si>
-    <t>hsphere_plan_7</t>
-  </si>
-  <si>
-    <t>hsphere_plan_8</t>
+    <t>hsphere_plan_10</t>
+  </si>
+  <si>
+    <t>hsphere_plan_11</t>
+  </si>
+  <si>
+    <t>hsphere_plan_12</t>
   </si>
 </sst>
 </file>
@@ -292,7 +301,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="17.88"/>
-    <col customWidth="1" min="6" max="6" width="15.13"/>
+    <col customWidth="1" min="2" max="2" width="17.5"/>
+    <col customWidth="1" min="3" max="3" width="18.75"/>
+    <col customWidth="1" min="4" max="4" width="17.5"/>
+    <col customWidth="1" min="8" max="8" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -314,45 +326,89 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>20.0</v>
+        <v>100.0</v>
       </c>
       <c r="C2" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="E2" s="1">
         <v>1.0</v>
       </c>
-      <c r="D2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3.0</v>
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
-        <v>25.0</v>
+        <v>50.0</v>
       </c>
       <c r="C3" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="E3" s="1">
         <v>2.0</v>
       </c>
-      <c r="D3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>150.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="E4" s="1">
         <v>3.0</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mapping opspi product id and hsphere plan id in csv file
</commit_message>
<xml_diff>
--- a/deployments/hsphere_plan_data.xlsx
+++ b/deployments/hsphere_plan_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>plan_name</t>
   </si>
@@ -37,20 +37,32 @@
     <t>opspi_account_id</t>
   </si>
   <si>
-    <t>hsphere_plan_10</t>
-  </si>
-  <si>
-    <t>hsphere_plan_11</t>
-  </si>
-  <si>
-    <t>hsphere_plan_12</t>
+    <t>hsphere_plan_id</t>
+  </si>
+  <si>
+    <t>hsphere_user_plan_2</t>
+  </si>
+  <si>
+    <t>hsphere_user_plan_3</t>
+  </si>
+  <si>
+    <t>hsphere_user_plan_4</t>
+  </si>
+  <si>
+    <t>hsphere_user_plan_5</t>
+  </si>
+  <si>
+    <t>hsphere_user_plan_6</t>
+  </si>
+  <si>
+    <t>hsphere_user_plan_7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -61,6 +73,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,12 +93,27 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -305,6 +336,7 @@
     <col customWidth="1" min="3" max="3" width="18.75"/>
     <col customWidth="1" min="4" max="4" width="17.5"/>
     <col customWidth="1" min="8" max="8" width="15.13"/>
+    <col customWidth="1" min="9" max="9" width="16.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -332,10 +364,13 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>100.0</v>
@@ -356,12 +391,15 @@
         <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>1.0</v>
+        <v>5.0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1234.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>50.0</v>
@@ -373,7 +411,7 @@
         <v>600.0</v>
       </c>
       <c r="E3" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
@@ -382,34 +420,165 @@
         <v>1</v>
       </c>
       <c r="H3" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2112.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>500.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="E4" s="3">
         <v>1.0</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>150.0</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3542.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="C5" s="3">
         <v>300.0</v>
       </c>
-      <c r="E4" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="F4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="D5" s="3">
+        <v>600.0</v>
+      </c>
+      <c r="E5" s="3">
         <v>1.0</v>
       </c>
+      <c r="F5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>4532.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>500.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>5643.0</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>300.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>600.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>6787.0</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>